<commit_message>
Role User Correction And Some Minor Corrections
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -31,66 +31,24 @@
     <t>bowling_style</t>
   </si>
   <si>
-    <t>Fakhar Zaman</t>
-  </si>
-  <si>
     <t>batsmen</t>
   </si>
   <si>
     <t>left</t>
   </si>
   <si>
-    <t>Abid Ali</t>
-  </si>
-  <si>
     <t>right</t>
   </si>
   <si>
-    <t>Muhammad Hafeez</t>
-  </si>
-  <si>
     <t>all-rounder</t>
   </si>
   <si>
-    <t>Shoaib Malik</t>
-  </si>
-  <si>
-    <t>Sarfaraz Ahmed</t>
-  </si>
-  <si>
     <t>wicket-keeper</t>
   </si>
   <si>
-    <t>Umar Akmal</t>
-  </si>
-  <si>
-    <t>Shadab Khan</t>
-  </si>
-  <si>
-    <t>Faheem Ashraf</t>
-  </si>
-  <si>
-    <t>Muhammad Aamir</t>
-  </si>
-  <si>
     <t>bowler</t>
   </si>
   <si>
-    <t>Junaid Khan</t>
-  </si>
-  <si>
-    <t>Usman Khan</t>
-  </si>
-  <si>
-    <t>Imam ul Haq</t>
-  </si>
-  <si>
-    <t>Shaheen Shinwari</t>
-  </si>
-  <si>
-    <t>Imad Wasim</t>
-  </si>
-  <si>
     <t>batting_hand</t>
   </si>
   <si>
@@ -119,6 +77,48 @@
   </si>
   <si>
     <t>left arm fast medium</t>
+  </si>
+  <si>
+    <t>Vince</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Cena</t>
+  </si>
+  <si>
+    <t>Orton</t>
+  </si>
+  <si>
+    <t>Reins</t>
+  </si>
+  <si>
+    <t>Rollins</t>
+  </si>
+  <si>
+    <t>Streather</t>
+  </si>
+  <si>
+    <t>Anrew</t>
+  </si>
+  <si>
+    <t>Micheal</t>
+  </si>
+  <si>
+    <t>Jordon</t>
+  </si>
+  <si>
+    <t>Obama</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>Heymen</t>
   </si>
 </sst>
 </file>
@@ -951,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -978,7 +978,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -987,296 +987,296 @@
     </row>
     <row r="2" spans="1:9" ht="30">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="30">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1">
         <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="30">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1">
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="30">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1">
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="30">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1">
         <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="30">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>96</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="30">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1">
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="45">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1">
         <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="30">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1">
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="30">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>83</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="30">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1">
         <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="30">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1">
         <v>88</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="30">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1">
         <v>73</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="30">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1">
         <v>51</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G15" s="2"/>
     </row>

</xml_diff>